<commit_message>
minor change in text on introduction
</commit_message>
<xml_diff>
--- a/SymbolSheetSecure.xlsx
+++ b/SymbolSheetSecure.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/johanfit/CloudStation/School/latex/Symbollist-maintain/symbollist-maintain-excel/Symbollist-maintain/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE1536F9-35A2-D84E-8EDC-6E9675709B45}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C6886E7-F836-A34E-90B5-05E12637924E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{C3287152-8E58-F540-9977-43335A6FB218}"/>
   </bookViews>
@@ -1029,8 +1029,8 @@
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>762000</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>139700</xdr:rowOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1046,7 +1046,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="88900" y="63500"/>
-          <a:ext cx="8102600" cy="4546600"/>
+          <a:ext cx="8102600" cy="4965700"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1674,7 +1674,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2653,7 +2653,7 @@
   <sheetPr codeName="Blad1"/>
   <dimension ref="A1:M101"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="A102" sqref="A102"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Some minor changes for making things more clear for user
</commit_message>
<xml_diff>
--- a/SymbolSheetSecure.xlsx
+++ b/SymbolSheetSecure.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/johanfit/CloudStation/School/latex/Symbollist-maintain/symbollist-maintain-excel/Symbollist-maintain/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EC784AC-FA3E-8B4F-9632-EA9B6FD4ADF3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDC942E5-47E5-2D48-92F6-34E6B4276027}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{C3287152-8E58-F540-9977-43335A6FB218}"/>
   </bookViews>
@@ -1707,11 +1707,12 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+      <selection activeCell="L21" sqref="L21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData/>
+  <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>